<commit_message>
most up to date changes
</commit_message>
<xml_diff>
--- a/Bill of Materials-RPD_top.xlsx
+++ b/Bill of Materials-RPD_top.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\AD17\2018 RPDU\trunk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE78FBB8-3359-4869-BCF3-3E99C14F18A4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D413D33B-6A72-4096-B86C-CA0B8040F5DB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11010" windowHeight="9915" xr2:uid="{7161A1E8-91F6-4A9D-AA41-5F325971F489}"/>
   </bookViews>
   <sheets>
     <sheet name="Board_use_vs_stock" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -208,9 +207,6 @@
     <t>usb header</t>
   </si>
   <si>
-    <t>MC74ACT125DTR2GOSDKR-ND</t>
-  </si>
-  <si>
     <t>MCP2515-I/SO-ND</t>
   </si>
   <si>
@@ -275,37 +271,19 @@
   </si>
   <si>
     <t>16.9k resistor</t>
+  </si>
+  <si>
+    <t>MC74ACT125DR2GOSDKR-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -332,23 +310,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -361,7 +328,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -423,39 +390,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="4" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Bad" xfId="3" builtinId="27"/>
-    <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
-    <cellStyle name="Good" xfId="2" builtinId="26"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -770,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441A0EE7-62CA-4107-A1F5-7FC9732F1640}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,839 +754,839 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="8">
-        <v>2</v>
-      </c>
-      <c r="D3" s="8">
-        <v>1</v>
-      </c>
-      <c r="E3" s="8">
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
         <f>2*C3-D3</f>
         <v>3</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="1">
         <v>3</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>7</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>16</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>9</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>17</v>
       </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2"/>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="1">
         <v>12</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="1">
         <v>12</v>
       </c>
-      <c r="E6" s="8">
-        <f t="shared" ref="E6:E35" si="0">2*C6-D6</f>
+      <c r="E6" s="1">
+        <f t="shared" ref="E6:E34" si="0">2*C6-D6</f>
         <v>12</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="1">
         <v>20</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="1">
         <v>4</v>
       </c>
-      <c r="D7" s="8">
-        <v>0</v>
-      </c>
-      <c r="E7" s="8">
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="1">
         <v>10</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="1">
         <v>3</v>
       </c>
-      <c r="D8" s="8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="8">
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="1">
         <v>10</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="2">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
         <v>8</v>
       </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2"/>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="8">
-        <v>1</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0</v>
-      </c>
-      <c r="E10" s="8">
-        <v>1</v>
-      </c>
-      <c r="F10" s="8">
-        <v>2</v>
-      </c>
-      <c r="G10" s="2"/>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="8">
-        <v>1</v>
-      </c>
-      <c r="D11" s="8">
-        <v>0</v>
-      </c>
-      <c r="E11" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F11" s="8">
-        <v>2</v>
-      </c>
-      <c r="G11" s="2"/>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="1">
         <v>9</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="1">
         <v>6</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="1">
         <v>12</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="1">
         <v>3</v>
       </c>
-      <c r="D13" s="8">
-        <v>0</v>
-      </c>
-      <c r="E13" s="8">
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="1">
         <v>10</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>4</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>26</v>
       </c>
-      <c r="E14" s="2">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2"/>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>5</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>14</v>
       </c>
-      <c r="E15" s="2">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0</v>
-      </c>
-      <c r="G15" s="2"/>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="1">
         <v>5</v>
       </c>
-      <c r="D16" s="8">
-        <v>0</v>
-      </c>
-      <c r="E16" s="8">
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="1">
         <v>10</v>
       </c>
-      <c r="G16" s="2"/>
+      <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="1">
         <v>3</v>
       </c>
-      <c r="D17" s="8">
-        <v>0</v>
-      </c>
-      <c r="E17" s="8">
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="1">
         <v>10</v>
       </c>
-      <c r="G17" s="2"/>
+      <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="8">
-        <v>1</v>
-      </c>
-      <c r="D18" s="8">
-        <v>0</v>
-      </c>
-      <c r="E18" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F18" s="8">
-        <v>2</v>
-      </c>
-      <c r="G18" s="2"/>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="8">
-        <v>1</v>
-      </c>
-      <c r="D19" s="8">
-        <v>0</v>
-      </c>
-      <c r="E19" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F19" s="8">
-        <v>2</v>
-      </c>
-      <c r="G19" s="2"/>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="8">
-        <v>2</v>
-      </c>
-      <c r="D20" s="8">
-        <v>0</v>
-      </c>
-      <c r="E20" s="8">
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="1">
         <v>4</v>
       </c>
-      <c r="G20" s="2"/>
+      <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="8">
-        <v>1</v>
-      </c>
-      <c r="D21" s="8">
-        <v>0</v>
-      </c>
-      <c r="E21" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F21" s="8">
-        <v>2</v>
-      </c>
-      <c r="G21" s="2"/>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="8">
-        <v>1</v>
-      </c>
-      <c r="D22" s="8">
-        <v>0</v>
-      </c>
-      <c r="E22" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F22" s="8">
-        <v>2</v>
-      </c>
-      <c r="G22" s="2"/>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="8">
-        <v>1</v>
-      </c>
-      <c r="D23" s="8">
-        <v>0</v>
-      </c>
-      <c r="E23" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F23" s="8">
-        <v>2</v>
-      </c>
-      <c r="G23" s="2"/>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="11" t="s">
+      <c r="A24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="12">
-        <v>2</v>
-      </c>
-      <c r="D24" s="12">
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
         <v>9</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="1">
         <f t="shared" si="0"/>
         <v>-5</v>
       </c>
-      <c r="F24" s="12">
-        <v>0</v>
-      </c>
-      <c r="G24" s="2"/>
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="2">
-        <v>2</v>
-      </c>
-      <c r="D25" s="2">
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
         <v>6</v>
       </c>
-      <c r="E25" s="2">
-        <v>0</v>
-      </c>
-      <c r="F25" s="2">
-        <v>0</v>
-      </c>
-      <c r="G25" s="2"/>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="8">
-        <v>1</v>
-      </c>
-      <c r="D26" s="8">
-        <v>0</v>
-      </c>
-      <c r="E26" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F26" s="8">
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F26" s="1">
         <v>4</v>
       </c>
-      <c r="G26" s="2"/>
+      <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="8">
-        <v>1</v>
-      </c>
-      <c r="D27" s="8">
-        <v>0</v>
-      </c>
-      <c r="E27" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F27" s="8">
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F27" s="1">
         <v>4</v>
       </c>
-      <c r="G27" s="2"/>
+      <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="8">
-        <v>1</v>
-      </c>
-      <c r="D28" s="8">
-        <v>0</v>
-      </c>
-      <c r="E28" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F28" s="8">
-        <v>2</v>
-      </c>
-      <c r="G28" s="2"/>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F28" s="1">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F29" s="1">
+        <v>2</v>
+      </c>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F30" s="1">
+        <v>2</v>
+      </c>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="8">
-        <v>1</v>
-      </c>
-      <c r="D29" s="8">
-        <v>0</v>
-      </c>
-      <c r="E29" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F29" s="8">
-        <v>2</v>
-      </c>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="B31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="8">
-        <v>1</v>
-      </c>
-      <c r="D30" s="8">
-        <v>0</v>
-      </c>
-      <c r="E30" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F30" s="8">
-        <v>2</v>
-      </c>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="8">
-        <v>1</v>
-      </c>
-      <c r="D31" s="8">
-        <v>0</v>
-      </c>
-      <c r="E31" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F31" s="8">
-        <v>2</v>
-      </c>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+      <c r="B32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="1">
+        <v>2</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F32" s="1">
+        <v>6</v>
+      </c>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F33" s="1">
+        <v>4</v>
+      </c>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="8">
-        <v>2</v>
-      </c>
-      <c r="D32" s="8">
-        <v>0</v>
-      </c>
-      <c r="E32" s="8">
-        <f t="shared" si="0"/>
+      <c r="B34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F34" s="1">
+        <v>5</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
+        <f>2*C35-D35</f>
+        <v>1</v>
+      </c>
+      <c r="F35" s="1">
+        <v>2</v>
+      </c>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="1">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1">
+        <v>8</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1">
         <v>4</v>
       </c>
-      <c r="F32" s="8">
-        <v>6</v>
-      </c>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" s="8">
-        <v>1</v>
-      </c>
-      <c r="D33" s="8">
-        <v>0</v>
-      </c>
-      <c r="E33" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F33" s="8">
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" ref="E38:E39" si="1">2*C38-D38</f>
         <v>4</v>
       </c>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="8">
-        <v>1</v>
-      </c>
-      <c r="D34" s="8">
-        <v>0</v>
-      </c>
-      <c r="E34" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F34" s="8">
-        <v>5</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" s="8">
-        <v>1</v>
-      </c>
-      <c r="D35" s="8">
-        <v>1</v>
-      </c>
-      <c r="E35" s="8">
-        <f>2*C35-D35</f>
-        <v>1</v>
-      </c>
-      <c r="F35" s="8">
-        <v>2</v>
-      </c>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36" s="2">
-        <v>2</v>
-      </c>
-      <c r="D36" s="2">
-        <v>8</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36" s="2">
-        <v>0</v>
-      </c>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="2">
-        <v>1</v>
-      </c>
-      <c r="D37" s="2">
-        <v>4</v>
-      </c>
-      <c r="E37" s="2">
-        <v>0</v>
-      </c>
-      <c r="F37" s="2">
-        <v>0</v>
-      </c>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B38" s="8" t="s">
+      <c r="F38" s="1">
+        <v>10</v>
+      </c>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="8">
-        <v>2</v>
-      </c>
-      <c r="D38" s="8">
-        <v>0</v>
-      </c>
-      <c r="E38" s="8">
-        <f t="shared" ref="E36:E39" si="1">2*C38-D38</f>
-        <v>4</v>
-      </c>
-      <c r="F38" s="8">
+      <c r="B39" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F39" s="1">
         <v>10</v>
       </c>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="8">
-        <v>1</v>
-      </c>
-      <c r="D39" s="8">
-        <v>0</v>
-      </c>
-      <c r="E39" s="8">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F39" s="8">
-        <v>10</v>
-      </c>
-      <c r="G39" s="2"/>
+      <c r="G39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>